<commit_message>
trailing stop loss updated
</commit_message>
<xml_diff>
--- a/Stock.xlsx
+++ b/Stock.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cskck\Desktop\Stock_Related\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cskck\Desktop\Stock_Related\Git_Repo\watchMyportfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB78899-E9B4-4CB3-A3E4-80D0B1467F52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C423944-FE19-4B37-912D-A40B2621D3EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F4941CB5-5CA2-47F4-BE77-B88332AD75D0}"/>
   </bookViews>
@@ -1165,7 +1165,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="P2" s="37">
         <f>SUM(P4:P1000)</f>
-        <v>-11712.85</v>
+        <v>-9832.85</v>
       </c>
       <c r="Q2" s="39"/>
     </row>
@@ -1311,7 +1311,7 @@
         <v>420</v>
       </c>
       <c r="G4" s="51">
-        <v>420</v>
+        <v>655</v>
       </c>
       <c r="H4" s="50">
         <f>IF((F4)="","",(CEILING((E4+((E4-F4)*2)),0.05)))</f>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="I4" s="3">
         <f>IFERROR(IF(L4="",(G4-E4)/E4,""),"")</f>
-        <v>-0.37369519832985387</v>
+        <v>-2.3262749776319747E-2</v>
       </c>
       <c r="J4" s="3">
         <f>IFERROR(IF(L4="",(H4-E4)/E4,""),"")</f>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="P4" s="2">
         <f>IF(B4="Open",((G4-E4)*D4),"")</f>
-        <v>-2004.8000000000002</v>
+        <v>-124.80000000000018</v>
       </c>
       <c r="Q4" s="11">
         <f t="shared" ref="Q4:Q67" si="4">IF(A4="","",A4)</f>

</xml_diff>

<commit_message>
Traliling stop loss changed
</commit_message>
<xml_diff>
--- a/Stock.xlsx
+++ b/Stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cskck\Desktop\Stock_Related\Git_Repo\watchMyportfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C423944-FE19-4B37-912D-A40B2621D3EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13473070-DF49-45A3-A170-2A23093733D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F4941CB5-5CA2-47F4-BE77-B88332AD75D0}"/>
   </bookViews>
@@ -1165,7 +1165,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="P2" s="37">
         <f>SUM(P4:P1000)</f>
-        <v>-9832.85</v>
+        <v>-7622.85</v>
       </c>
       <c r="Q2" s="39"/>
     </row>
@@ -1311,7 +1311,7 @@
         <v>420</v>
       </c>
       <c r="G4" s="51">
-        <v>655</v>
+        <v>800</v>
       </c>
       <c r="H4" s="50">
         <f>IF((F4)="","",(CEILING((E4+((E4-F4)*2)),0.05)))</f>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="I4" s="3">
         <f>IFERROR(IF(L4="",(G4-E4)/E4,""),"")</f>
-        <v>-2.3262749776319747E-2</v>
+        <v>0.1929615269907545</v>
       </c>
       <c r="J4" s="3">
         <f>IFERROR(IF(L4="",(H4-E4)/E4,""),"")</f>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="P4" s="2">
         <f>IF(B4="Open",((G4-E4)*D4),"")</f>
-        <v>-124.80000000000018</v>
+        <v>1035.1999999999998</v>
       </c>
       <c r="Q4" s="11">
         <f t="shared" ref="Q4:Q67" si="4">IF(A4="","",A4)</f>
@@ -1367,7 +1367,7 @@
         <v>3150</v>
       </c>
       <c r="G5" s="51">
-        <v>3150</v>
+        <v>3500</v>
       </c>
       <c r="H5" s="50">
         <f t="shared" ref="H5:H68" si="5">IF((F5)="","",(CEILING((E5+((E5-F5)*2)),0.05)))</f>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="I5" s="3">
         <f t="shared" ref="I5:I68" si="6">IFERROR(IF(L5="",(G5-E5)/E5,""),"")</f>
-        <v>-0.16598268421191986</v>
+        <v>-7.3314093568799837E-2</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ref="J5:J68" si="7">IFERROR(IF(L5="",(H5-E5)/E5,""),"")</f>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="P5" s="2">
         <f t="shared" ref="P5:P13" si="9">IF(B5="Open",((G5-E5)*D5),"")</f>
-        <v>-1880.7000000000003</v>
+        <v>-830.70000000000027</v>
       </c>
       <c r="Q5" s="11">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
added filter for only open stocks
</commit_message>
<xml_diff>
--- a/Stock.xlsx
+++ b/Stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cskck\Desktop\Stock_Related\Git_Repo\watchMyportfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13473070-DF49-45A3-A170-2A23093733D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF67E08-CB28-47B0-8D59-14A7EEEB72B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F4941CB5-5CA2-47F4-BE77-B88332AD75D0}"/>
   </bookViews>
@@ -1165,7 +1165,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,16 +1226,16 @@
       <c r="L2" s="34"/>
       <c r="M2" s="37">
         <f t="shared" ref="M2" si="0">SUM(M4:M1000)</f>
-        <v>0</v>
+        <v>-2013.9000000000003</v>
       </c>
       <c r="N2" s="37"/>
       <c r="O2" s="38">
         <f>SUM(O4:O1000)</f>
-        <v>38872.850000000006</v>
+        <v>31305.850000000002</v>
       </c>
       <c r="P2" s="37">
         <f>SUM(P4:P1000)</f>
-        <v>-7622.85</v>
+        <v>-5655.85</v>
       </c>
       <c r="Q2" s="39"/>
     </row>
@@ -1576,7 +1576,7 @@
       </c>
       <c r="B9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Open</v>
+        <v>Closed</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>33</v>
@@ -1597,29 +1597,35 @@
         <f t="shared" si="5"/>
         <v>821.5</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>-0.25994449583718782</v>
-      </c>
-      <c r="J9" s="3">
+        <v/>
+      </c>
+      <c r="J9" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>0.51988899167437563</v>
-      </c>
-      <c r="M9" s="4" t="str">
+        <v/>
+      </c>
+      <c r="K9" s="31">
+        <v>44616</v>
+      </c>
+      <c r="L9" s="30">
+        <v>396.65</v>
+      </c>
+      <c r="M9" s="4">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N9" s="3" t="str">
+        <v>-2013.9000000000003</v>
+      </c>
+      <c r="N9" s="3">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="O9" s="5">
+        <v>-0.26614246068455139</v>
+      </c>
+      <c r="O9" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>7567</v>
-      </c>
-      <c r="P9" s="2">
+        <v/>
+      </c>
+      <c r="P9" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>-1967</v>
+        <v/>
       </c>
       <c r="Q9" s="11">
         <f>IF(A9="","",A9)</f>

</xml_diff>

<commit_message>
change the stop loss for UNIVPHOTO
</commit_message>
<xml_diff>
--- a/Stock.xlsx
+++ b/Stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cskck\Desktop\Stock_Related\Git_Repo\watchMyportfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF67E08-CB28-47B0-8D59-14A7EEEB72B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022FA8E7-E8CD-4433-8C76-1A5CCD9B050C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F4941CB5-5CA2-47F4-BE77-B88332AD75D0}"/>
   </bookViews>
@@ -1165,7 +1165,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="P2" s="37">
         <f>SUM(P4:P1000)</f>
-        <v>-5655.85</v>
+        <v>-8695.85</v>
       </c>
       <c r="Q2" s="39"/>
     </row>
@@ -1311,7 +1311,7 @@
         <v>420</v>
       </c>
       <c r="G4" s="51">
-        <v>800</v>
+        <v>420</v>
       </c>
       <c r="H4" s="50">
         <f>IF((F4)="","",(CEILING((E4+((E4-F4)*2)),0.05)))</f>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="I4" s="3">
         <f>IFERROR(IF(L4="",(G4-E4)/E4,""),"")</f>
-        <v>0.1929615269907545</v>
+        <v>-0.37369519832985387</v>
       </c>
       <c r="J4" s="3">
         <f>IFERROR(IF(L4="",(H4-E4)/E4,""),"")</f>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="P4" s="2">
         <f>IF(B4="Open",((G4-E4)*D4),"")</f>
-        <v>1035.1999999999998</v>
+        <v>-2004.8000000000002</v>
       </c>
       <c r="Q4" s="11">
         <f t="shared" ref="Q4:Q67" si="4">IF(A4="","",A4)</f>

</xml_diff>